<commit_message>
Added US07 , US08 and TM07
</commit_message>
<xml_diff>
--- a/Testplan Rapport mm/Matris - User Stories - FyraiRad - Case 2 Sprint 1.xlsx
+++ b/Testplan Rapport mm/Matris - User Stories - FyraiRad - Case 2 Sprint 1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4843D7-6B43-4192-B857-D5C18E940016}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FB69B8-5799-48C1-8F06-EE4BFE7379DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>US01</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>As a user I want to be able to change the avatar, so I can look the way I want too</t>
+  </si>
+  <si>
+    <t>US07</t>
+  </si>
+  <si>
+    <t>As a user I want to know how good this application's bots is compared to other applications</t>
+  </si>
+  <si>
+    <t>US08</t>
+  </si>
+  <si>
+    <t>As a user I want the application to be stable so that my game doesn't get interrupted</t>
+  </si>
+  <si>
+    <t>TM07</t>
   </si>
 </sst>
 </file>
@@ -531,28 +546,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB38"/>
+  <dimension ref="A1:AC42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="14"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
@@ -568,23 +587,26 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="N2" s="4"/>
-      <c r="U2" s="1"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="1"/>
+      <c r="K2" s="14"/>
+      <c r="O2" s="4"/>
+      <c r="V2" s="1"/>
+      <c r="X2" s="2"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -596,18 +618,16 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="23" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="W3" s="5"/>
-    </row>
-    <row r="4" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -617,18 +637,16 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="19"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L4" s="14"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="4"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>20</v>
@@ -640,19 +658,18 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="23" t="s">
+      <c r="J5" s="19"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>21</v>
@@ -664,16 +681,17 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="14"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="10"/>
-      <c r="O6" s="6"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="10"/>
       <c r="P6" s="6"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="6"/>
       <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -685,16 +703,17 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="21"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="13"/>
-      <c r="O7" s="7"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="13"/>
       <c r="P7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -706,247 +725,232 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="6"/>
-      <c r="R8" s="7"/>
+      <c r="O8" s="6"/>
       <c r="S8" s="7"/>
-    </row>
-    <row r="9" spans="1:28" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="22"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="19"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="6"/>
-      <c r="R9" s="7"/>
+      <c r="O9" s="6"/>
       <c r="S9" s="7"/>
-    </row>
-    <row r="10" spans="1:28" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="6"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="3"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-    </row>
-    <row r="11" spans="1:28" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O10" s="6"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:29" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="4"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-    </row>
-    <row r="12" spans="1:28" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="6"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="14"/>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="1"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="3"/>
+      <c r="V12" s="4"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="7"/>
+      <c r="X12" s="6"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC12" s="7"/>
+    </row>
+    <row r="13" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="6"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
+      <c r="O13" s="6"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="1"/>
-      <c r="U13" s="6"/>
+      <c r="S13" s="7"/>
+      <c r="V13" s="4"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="7"/>
+      <c r="X13" s="6"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
-    </row>
-    <row r="14" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC13" s="7"/>
+    </row>
+    <row r="14" spans="1:29" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="6"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="7"/>
+      <c r="O14" s="6"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="1"/>
-      <c r="U14" s="11"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="1"/>
+      <c r="V14" s="4"/>
       <c r="W14" s="6"/>
-      <c r="X14" s="7"/>
+      <c r="X14" s="6"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
-    </row>
-    <row r="15" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC14" s="7"/>
+    </row>
+    <row r="15" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>13</v>
-      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="14"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="6"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="7"/>
+      <c r="O15" s="6"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="1"/>
-      <c r="U15" s="11"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="1"/>
+      <c r="V15" s="6"/>
+      <c r="X15" s="6"/>
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
-    </row>
-    <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC15" s="7"/>
+    </row>
+    <row r="16" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="14"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="6"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="4"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="7"/>
+      <c r="O16" s="6"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="1"/>
-      <c r="U16" s="11"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="1"/>
+      <c r="V16" s="11"/>
+      <c r="X16" s="6"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
-    </row>
-    <row r="17" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC16" s="7"/>
+    </row>
+    <row r="17" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="21"/>
@@ -954,137 +958,164 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="6"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="6"/>
-      <c r="O17" s="7"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="1"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="1"/>
+      <c r="V17" s="11"/>
+      <c r="X17" s="6"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
-    </row>
-    <row r="18" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC17" s="7"/>
+    </row>
+    <row r="18" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="14"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="1"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-    </row>
-    <row r="19" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="14"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="1"/>
+      <c r="V18" s="11"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+    </row>
+    <row r="19" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="1"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="6"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="6"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="1"/>
+      <c r="V19" s="4"/>
       <c r="W19" s="6"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-    </row>
-    <row r="20" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="6"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+    </row>
+    <row r="20" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+        <v>22</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="U20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="6"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="1"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
-    </row>
-    <row r="21" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC20" s="6"/>
+    </row>
+    <row r="21" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+        <v>15</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
-      <c r="U21" s="4"/>
-      <c r="AB21" s="7"/>
-    </row>
-    <row r="22" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="14"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="1"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+    </row>
+    <row r="22" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -1096,15 +1127,17 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="14"/>
+      <c r="V22" s="4"/>
+      <c r="AC22" s="6"/>
+    </row>
+    <row r="23" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -1116,23 +1149,83 @@
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="14"/>
+      <c r="V23" s="4"/>
+      <c r="AC23" s="6"/>
+    </row>
+    <row r="24" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
-    </row>
-    <row r="25" spans="1:28" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="V24" s="4"/>
+      <c r="AC24" s="6"/>
+    </row>
+    <row r="25" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="V25" s="7"/>
-      <c r="X25" s="10"/>
-    </row>
-    <row r="26" spans="1:28" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="V25" s="4"/>
+      <c r="AC25" s="7"/>
+    </row>
+    <row r="26" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="V26" s="7"/>
-      <c r="X26" s="10"/>
-    </row>
-    <row r="27" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
@@ -1143,18 +1236,35 @@
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
-    </row>
-    <row r="31" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-    </row>
-    <row r="32" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-    </row>
-    <row r="33" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-    </row>
-    <row r="34" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="29" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="W29" s="7"/>
+      <c r="Y29" s="10"/>
+    </row>
+    <row r="30" spans="1:29" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="W30" s="7"/>
+      <c r="Y30" s="10"/>
+    </row>
+    <row r="31" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
     </row>
     <row r="35" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
@@ -1167,6 +1277,18 @@
     </row>
     <row r="38" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
+    </row>
+    <row r="39" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+    </row>
+    <row r="41" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>